<commit_message>
latihan tabel menambahkan jadwal prakerin dan daftar gambar
</commit_message>
<xml_diff>
--- a/REVISI JADWAL PRA PRAKRIN RPL.xlsx
+++ b/REVISI JADWAL PRA PRAKRIN RPL.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DOKUMEN\PRAKERIN\2024\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="75" windowWidth="16215" windowHeight="7935"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8655" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="REVISI" sheetId="1" r:id="rId1"/>
+    <sheet name="jadwal prakerin" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="64">
   <si>
     <t>Minggu 1</t>
   </si>
@@ -137,13 +143,82 @@
   </si>
   <si>
     <t>Cara menghadapi atasan dan rekan kerja online dan offline</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Uraian Kegiatan</t>
+  </si>
+  <si>
+    <t>Tempat</t>
+  </si>
+  <si>
+    <t>Bulan</t>
+  </si>
+  <si>
+    <t>Juli</t>
+  </si>
+  <si>
+    <t>Agustus</t>
+  </si>
+  <si>
+    <t>September</t>
+  </si>
+  <si>
+    <t>Oktober</t>
+  </si>
+  <si>
+    <t>November</t>
+  </si>
+  <si>
+    <t>Desember</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Persiapan </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sekolah </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pengantaran </t>
+  </si>
+  <si>
+    <t xml:space="preserve">perkenalan/Adaptasi </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tempat PKL </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Analisis masalah </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Merancang database </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mreancang UX/UI </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mengetik source code </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uji coba aplikas/debugging </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Evaluasi </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kegiatan Rutin Harian Kantor </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Penjemputan </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -151,6 +226,31 @@
       <family val="2"/>
       <charset val="1"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -212,7 +312,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -221,12 +321,38 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -273,7 +399,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -305,9 +431,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -339,6 +466,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -514,14 +642,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:S22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="9.140625" customWidth="1"/>
     <col min="4" max="4" width="6.140625" customWidth="1"/>
@@ -530,7 +658,7 @@
     <col min="16" max="16" width="5.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -557,7 +685,7 @@
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -604,7 +732,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -647,7 +775,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -694,7 +822,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
@@ -741,7 +869,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
@@ -788,7 +916,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>22</v>
       </c>
@@ -835,7 +963,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
@@ -882,7 +1010,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E14" s="5" t="s">
         <v>29</v>
       </c>
@@ -890,7 +1018,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
         <v>31</v>
       </c>
@@ -899,7 +1027,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
         <v>33</v>
       </c>
@@ -907,32 +1035,32 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="9:9">
+    <row r="17" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I17" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="9:9">
+    <row r="18" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I18" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="9:9">
+    <row r="19" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I19" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="9:9">
+    <row r="20" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I20" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="9:9">
+    <row r="21" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I21" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="9:9">
+    <row r="22" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I22" t="s">
         <v>40</v>
       </c>
@@ -941,4 +1069,627 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:AD16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="160" zoomScaleNormal="145" zoomScaleSheetLayoutView="160" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.85546875" style="8" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" style="8" customWidth="1"/>
+    <col min="4" max="30" width="1.7109375" style="8" customWidth="1"/>
+    <col min="31" max="16384" width="9.140625" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="9"/>
+      <c r="T3" s="9"/>
+      <c r="U3" s="9"/>
+      <c r="V3" s="9"/>
+      <c r="W3" s="9"/>
+      <c r="X3" s="9"/>
+      <c r="Y3" s="9"/>
+      <c r="Z3" s="9"/>
+      <c r="AA3" s="9"/>
+      <c r="AB3" s="9"/>
+      <c r="AC3" s="9"/>
+      <c r="AD3" s="9"/>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="R4" s="9"/>
+      <c r="S4" s="9"/>
+      <c r="T4" s="9"/>
+      <c r="U4" s="9"/>
+      <c r="V4" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="W4" s="9"/>
+      <c r="X4" s="9"/>
+      <c r="Y4" s="9"/>
+      <c r="Z4" s="9"/>
+      <c r="AA4" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB4" s="9"/>
+      <c r="AC4" s="9"/>
+      <c r="AD4" s="9"/>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="13">
+        <v>1</v>
+      </c>
+      <c r="E5" s="13">
+        <v>2</v>
+      </c>
+      <c r="F5" s="13">
+        <v>3</v>
+      </c>
+      <c r="G5" s="13">
+        <v>4</v>
+      </c>
+      <c r="H5" s="13">
+        <v>5</v>
+      </c>
+      <c r="I5" s="13">
+        <v>1</v>
+      </c>
+      <c r="J5" s="13">
+        <v>2</v>
+      </c>
+      <c r="K5" s="13">
+        <v>3</v>
+      </c>
+      <c r="L5" s="13">
+        <v>4</v>
+      </c>
+      <c r="M5" s="13">
+        <v>1</v>
+      </c>
+      <c r="N5" s="13">
+        <v>2</v>
+      </c>
+      <c r="O5" s="13">
+        <v>3</v>
+      </c>
+      <c r="P5" s="13">
+        <v>4</v>
+      </c>
+      <c r="Q5" s="13">
+        <v>1</v>
+      </c>
+      <c r="R5" s="13">
+        <v>2</v>
+      </c>
+      <c r="S5" s="13">
+        <v>3</v>
+      </c>
+      <c r="T5" s="13">
+        <v>4</v>
+      </c>
+      <c r="U5" s="13">
+        <v>5</v>
+      </c>
+      <c r="V5" s="13">
+        <v>1</v>
+      </c>
+      <c r="W5" s="13">
+        <v>2</v>
+      </c>
+      <c r="X5" s="13">
+        <v>3</v>
+      </c>
+      <c r="Y5" s="13">
+        <v>4</v>
+      </c>
+      <c r="Z5" s="13">
+        <v>5</v>
+      </c>
+      <c r="AA5" s="13">
+        <v>1</v>
+      </c>
+      <c r="AB5" s="13">
+        <v>2</v>
+      </c>
+      <c r="AC5" s="13">
+        <v>3</v>
+      </c>
+      <c r="AD5" s="13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
+        <v>1</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" s="12"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="13"/>
+      <c r="R6" s="13"/>
+      <c r="S6" s="13"/>
+      <c r="T6" s="13"/>
+      <c r="U6" s="13"/>
+      <c r="V6" s="13"/>
+      <c r="W6" s="13"/>
+      <c r="X6" s="13"/>
+      <c r="Y6" s="13"/>
+      <c r="Z6" s="13"/>
+      <c r="AA6" s="13"/>
+      <c r="AB6" s="13"/>
+      <c r="AC6" s="13"/>
+      <c r="AD6" s="13"/>
+    </row>
+    <row r="7" spans="1:30" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="10">
+        <v>2</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" s="13"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13"/>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="13"/>
+      <c r="R7" s="13"/>
+      <c r="S7" s="13"/>
+      <c r="T7" s="13"/>
+      <c r="U7" s="13"/>
+      <c r="V7" s="13"/>
+      <c r="W7" s="13"/>
+      <c r="X7" s="13"/>
+      <c r="Y7" s="13"/>
+      <c r="Z7" s="13"/>
+      <c r="AA7" s="13"/>
+      <c r="AB7" s="13"/>
+      <c r="AC7" s="13"/>
+      <c r="AD7" s="13"/>
+    </row>
+    <row r="8" spans="1:30" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="10">
+        <v>3</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="13"/>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="13"/>
+      <c r="R8" s="13"/>
+      <c r="S8" s="13"/>
+      <c r="T8" s="13"/>
+      <c r="U8" s="13"/>
+      <c r="V8" s="13"/>
+      <c r="W8" s="13"/>
+      <c r="X8" s="13"/>
+      <c r="Y8" s="13"/>
+      <c r="Z8" s="13"/>
+      <c r="AA8" s="13"/>
+      <c r="AB8" s="13"/>
+      <c r="AC8" s="13"/>
+      <c r="AD8" s="13"/>
+    </row>
+    <row r="9" spans="1:30" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="10">
+        <v>4</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="13"/>
+      <c r="R9" s="13"/>
+      <c r="S9" s="13"/>
+      <c r="T9" s="13"/>
+      <c r="U9" s="13"/>
+      <c r="V9" s="13"/>
+      <c r="W9" s="13"/>
+      <c r="X9" s="13"/>
+      <c r="Y9" s="13"/>
+      <c r="Z9" s="13"/>
+      <c r="AA9" s="13"/>
+      <c r="AB9" s="13"/>
+      <c r="AC9" s="13"/>
+      <c r="AD9" s="13"/>
+    </row>
+    <row r="10" spans="1:30" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="10">
+        <v>5</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="13"/>
+      <c r="R10" s="13"/>
+      <c r="S10" s="13"/>
+      <c r="T10" s="13"/>
+      <c r="U10" s="13"/>
+      <c r="V10" s="13"/>
+      <c r="W10" s="13"/>
+      <c r="X10" s="13"/>
+      <c r="Y10" s="13"/>
+      <c r="Z10" s="13"/>
+      <c r="AA10" s="13"/>
+      <c r="AB10" s="13"/>
+      <c r="AC10" s="13"/>
+      <c r="AD10" s="13"/>
+    </row>
+    <row r="11" spans="1:30" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10">
+        <v>6</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="13"/>
+      <c r="P11" s="13"/>
+      <c r="Q11" s="13"/>
+      <c r="R11" s="13"/>
+      <c r="S11" s="13"/>
+      <c r="T11" s="13"/>
+      <c r="U11" s="13"/>
+      <c r="V11" s="13"/>
+      <c r="W11" s="13"/>
+      <c r="X11" s="13"/>
+      <c r="Y11" s="13"/>
+      <c r="Z11" s="13"/>
+      <c r="AA11" s="13"/>
+      <c r="AB11" s="13"/>
+      <c r="AC11" s="13"/>
+      <c r="AD11" s="13"/>
+    </row>
+    <row r="12" spans="1:30" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="10">
+        <v>7</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="12"/>
+      <c r="P12" s="12"/>
+      <c r="Q12" s="12"/>
+      <c r="R12" s="12"/>
+      <c r="S12" s="12"/>
+      <c r="T12" s="12"/>
+      <c r="U12" s="12"/>
+      <c r="V12" s="12"/>
+      <c r="W12" s="13"/>
+      <c r="X12" s="13"/>
+      <c r="Y12" s="13"/>
+      <c r="Z12" s="13"/>
+      <c r="AA12" s="13"/>
+      <c r="AB12" s="13"/>
+      <c r="AC12" s="13"/>
+      <c r="AD12" s="13"/>
+    </row>
+    <row r="13" spans="1:30" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10">
+        <v>8</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="13"/>
+      <c r="P13" s="12"/>
+      <c r="Q13" s="12"/>
+      <c r="R13" s="12"/>
+      <c r="S13" s="12"/>
+      <c r="T13" s="12"/>
+      <c r="U13" s="12"/>
+      <c r="V13" s="12"/>
+      <c r="W13" s="12"/>
+      <c r="X13" s="12"/>
+      <c r="Y13" s="12"/>
+      <c r="Z13" s="12"/>
+      <c r="AA13" s="12"/>
+      <c r="AB13" s="13"/>
+      <c r="AC13" s="13"/>
+      <c r="AD13" s="13"/>
+    </row>
+    <row r="14" spans="1:30" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="10">
+        <v>9</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="12"/>
+      <c r="P14" s="12"/>
+      <c r="Q14" s="12"/>
+      <c r="R14" s="12"/>
+      <c r="S14" s="12"/>
+      <c r="T14" s="12"/>
+      <c r="U14" s="12"/>
+      <c r="V14" s="12"/>
+      <c r="W14" s="12"/>
+      <c r="X14" s="12"/>
+      <c r="Y14" s="12"/>
+      <c r="Z14" s="12"/>
+      <c r="AA14" s="12"/>
+      <c r="AB14" s="12"/>
+      <c r="AC14" s="12"/>
+      <c r="AD14" s="13"/>
+    </row>
+    <row r="15" spans="1:30" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="10">
+        <v>10</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="12"/>
+      <c r="P15" s="12"/>
+      <c r="Q15" s="12"/>
+      <c r="R15" s="12"/>
+      <c r="S15" s="12"/>
+      <c r="T15" s="12"/>
+      <c r="U15" s="12"/>
+      <c r="V15" s="12"/>
+      <c r="W15" s="12"/>
+      <c r="X15" s="12"/>
+      <c r="Y15" s="12"/>
+      <c r="Z15" s="12"/>
+      <c r="AA15" s="12"/>
+      <c r="AB15" s="12"/>
+      <c r="AC15" s="12"/>
+      <c r="AD15" s="13"/>
+    </row>
+    <row r="16" spans="1:30" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="10">
+        <v>11</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="13"/>
+      <c r="N16" s="13"/>
+      <c r="O16" s="13"/>
+      <c r="P16" s="13"/>
+      <c r="Q16" s="13"/>
+      <c r="R16" s="13"/>
+      <c r="S16" s="13"/>
+      <c r="T16" s="13"/>
+      <c r="U16" s="13"/>
+      <c r="V16" s="13"/>
+      <c r="W16" s="13"/>
+      <c r="X16" s="13"/>
+      <c r="Y16" s="13"/>
+      <c r="Z16" s="13"/>
+      <c r="AA16" s="13"/>
+      <c r="AB16" s="13"/>
+      <c r="AC16" s="13"/>
+      <c r="AD16" s="12"/>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="D3:AD3"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="AA4:AD4"/>
+    <mergeCell ref="V4:Z4"/>
+    <mergeCell ref="Q4:U4"/>
+    <mergeCell ref="M4:P4"/>
+    <mergeCell ref="I4:L4"/>
+    <mergeCell ref="D4:H4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>